<commit_message>
complete monthly and re-run daily
</commit_message>
<xml_diff>
--- a/Output/March/productivity_TL/productivity_TL_2022-03-01.xlsx
+++ b/Output/March/productivity_TL/productivity_TL_2022-03-01.xlsx
@@ -910,13 +910,13 @@
         <v>0</v>
       </c>
       <c r="S6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T6">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="U6">
-        <v>0.07692307692307693</v>
+        <v>0.09375</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -1267,10 +1267,10 @@
         <v>2</v>
       </c>
       <c r="T12">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="U12">
-        <v>0.09523809523809523</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -1506,13 +1506,13 @@
         <v>7.65</v>
       </c>
       <c r="F2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G2">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="H2">
-        <v>0.0851063829787234</v>
+        <v>0.08771929824561403</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1735,7 +1735,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>0.0851063829787234</v>
+        <v>0.08771929824561403</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1877,7 +1877,7 @@
         <v>47</v>
       </c>
       <c r="D2">
-        <v>0.0851063829787234</v>
+        <v>0.08771929824561403</v>
       </c>
       <c r="E2">
         <v>1</v>

</xml_diff>